<commit_message>
upd: periodic base update
</commit_message>
<xml_diff>
--- a/ministers.xlsx
+++ b/ministers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HAYKLID-PC\Documents\GitHub\Payment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1DB9219-D34C-4670-847F-0EC25A65DC2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9177F2BF-3D6E-4488-A5B1-6D00CCE2627B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1320" yWindow="345" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -20,87 +20,144 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="46">
+  <si>
+    <t>Родина Анастасия</t>
+  </si>
   <si>
     <t>9А</t>
   </si>
   <si>
+    <t>judgement</t>
+  </si>
+  <si>
+    <t>Коренюгина Екатерина</t>
+  </si>
+  <si>
+    <t>Икболова Алина</t>
+  </si>
+  <si>
+    <t>socdev</t>
+  </si>
+  <si>
+    <t>Безбородов Вадим</t>
+  </si>
+  <si>
+    <t>10В</t>
+  </si>
+  <si>
+    <t>Левина Виолетта</t>
+  </si>
+  <si>
+    <t>Юзефович Анастасия</t>
+  </si>
+  <si>
+    <t>Симошин Михаил</t>
+  </si>
+  <si>
     <t>economic</t>
   </si>
   <si>
+    <t>Шевченко Анастасия</t>
+  </si>
+  <si>
+    <t>Грибова Диана</t>
+  </si>
+  <si>
+    <t>10Б</t>
+  </si>
+  <si>
+    <t>Якшина Мария</t>
+  </si>
+  <si>
+    <t>Пирбудагова Лина</t>
+  </si>
+  <si>
+    <t>Чернавкин Максим</t>
+  </si>
+  <si>
+    <t>Денисов Максим</t>
+  </si>
+  <si>
     <t>mvd</t>
   </si>
   <si>
+    <t>Федотов Иван</t>
+  </si>
+  <si>
+    <t>Саломов Холид</t>
+  </si>
+  <si>
+    <t>Пронин Александр</t>
+  </si>
+  <si>
+    <t>Артёмов Игорь</t>
+  </si>
+  <si>
+    <t>Сибряев Константин</t>
+  </si>
+  <si>
+    <t>Ишмуратов Денис</t>
+  </si>
+  <si>
     <t>9A</t>
   </si>
   <si>
-    <t>judgement</t>
-  </si>
-  <si>
-    <t>10В</t>
-  </si>
-  <si>
-    <t>10Б</t>
-  </si>
-  <si>
-    <t>socdev</t>
-  </si>
-  <si>
-    <t>Родина Анастасия</t>
-  </si>
-  <si>
-    <t>Коренюгина Екатерина</t>
-  </si>
-  <si>
-    <t>Икболова Алина</t>
-  </si>
-  <si>
-    <t>Безбородов Вадим</t>
-  </si>
-  <si>
-    <t>Левина Виолетта</t>
-  </si>
-  <si>
-    <t>Юзефович Анастасия</t>
-  </si>
-  <si>
-    <t>Шевченко Анастасия</t>
-  </si>
-  <si>
-    <t>Грибова Диана</t>
-  </si>
-  <si>
-    <t>Якшина Мария</t>
-  </si>
-  <si>
-    <t>Пирбудагова Лина</t>
-  </si>
-  <si>
-    <t>Чернавкин Максим</t>
-  </si>
-  <si>
-    <t>Денисов Максим</t>
-  </si>
-  <si>
-    <t>Федотов Иван</t>
-  </si>
-  <si>
-    <t>Пронин Александр</t>
-  </si>
-  <si>
-    <t>Артёмов Игорь</t>
-  </si>
-  <si>
-    <t>Сибряев Константин</t>
-  </si>
-  <si>
-    <t>Ишмуратов Денис</t>
-  </si>
-  <si>
-    <t>Саломов Холид</t>
-  </si>
-  <si>
-    <t>Симошин Михаил</t>
+    <t>CFsmHWzYZq</t>
+  </si>
+  <si>
+    <t>YEZPDzXL1U</t>
+  </si>
+  <si>
+    <t>7Sns4P6WG3</t>
+  </si>
+  <si>
+    <t>H8MIla0Eeq</t>
+  </si>
+  <si>
+    <t>vdz6tDIsjQ</t>
+  </si>
+  <si>
+    <t>a01RBfPeWH</t>
+  </si>
+  <si>
+    <t>VPBl461QKo</t>
+  </si>
+  <si>
+    <t>FiNaBQEY0h</t>
+  </si>
+  <si>
+    <t>yBh8s5mAc7</t>
+  </si>
+  <si>
+    <t>9ljQC7BvmX</t>
+  </si>
+  <si>
+    <t>M6REuPDOim</t>
+  </si>
+  <si>
+    <t>aUHTui5MVR</t>
+  </si>
+  <si>
+    <t>AjboqdvkRx</t>
+  </si>
+  <si>
+    <t>41JxlYQqWg</t>
+  </si>
+  <si>
+    <t>0lkewEL78G</t>
+  </si>
+  <si>
+    <t>XaoC2w63jY</t>
+  </si>
+  <si>
+    <t>5s1jPEcQRx</t>
+  </si>
+  <si>
+    <t>nTVZ2a5XLG</t>
+  </si>
+  <si>
+    <t>8kpxUJ1Ojz</t>
   </si>
 </sst>
 </file>
@@ -435,229 +492,287 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="48.7109375" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="9.140625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="B6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="B7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="D8" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="C9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="B10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="B11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="B12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="B13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="B19" s="1" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>2</v>
+        <v>19</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>